<commit_message>
added all place holder slides and updated spreadsheet
</commit_message>
<xml_diff>
--- a/Delta & Databricks for the DBA.xlsx
+++ b/Delta & Databricks for the DBA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\delta-dbx-for-dba\delta-dbx-for-dba\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A51D8FF-74E6-4884-A276-AA7DF9E1F2E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A9E122B-F5D8-4A45-B9F4-730D79A6116A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51720" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{0EC3342C-DA2B-4212-93EF-7E4274CD2C90}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" xr2:uid="{0EC3342C-DA2B-4212-93EF-7E4274CD2C90}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="34">
   <si>
     <t>Delta/Databricks Feature</t>
   </si>
@@ -135,6 +135,9 @@
   </si>
   <si>
     <t xml:space="preserve">Identity Columns </t>
+  </si>
+  <si>
+    <t>Order</t>
   </si>
 </sst>
 </file>
@@ -502,238 +505,268 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{917A3BBD-93CA-4209-8D51-52271B5B056D}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="38.578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.578125" customWidth="1"/>
-    <col min="3" max="3" width="27.83984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.83984375" customWidth="1"/>
-    <col min="5" max="5" width="77.26171875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.578125" customWidth="1"/>
+    <col min="4" max="4" width="27.83984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.83984375" customWidth="1"/>
+    <col min="6" max="6" width="77.26171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
+      <c r="F10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" t="s">
+      <c r="F12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B13" t="s">
         <v>16</v>
       </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" t="s">
         <v>9</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" t="s">
-        <v>31</v>
-      </c>
-    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F13">
+    <sortCondition ref="A1:A13"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="549332d9-68bf-4487-9fc8-f898b54ba2f4">
@@ -742,6 +775,15 @@
     <TaxCatchAll xmlns="e5446278-f595-413d-97e8-9d05bced5ef2" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -988,20 +1030,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FA90A2C-ECC6-4D8A-8320-8A9430408ADD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1518E235-21CD-4DD0-8F51-C8B7F1A485C0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="549332d9-68bf-4487-9fc8-f898b54ba2f4"/>
     <ds:schemaRef ds:uri="e5446278-f595-413d-97e8-9d05bced5ef2"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FA90A2C-ECC6-4D8A-8320-8A9430408ADD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
lastes changes to ppt
</commit_message>
<xml_diff>
--- a/Delta & Databricks for the DBA.xlsx
+++ b/Delta & Databricks for the DBA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\delta-dbx-for-dba\delta-dbx-for-dba\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A9E122B-F5D8-4A45-B9F4-730D79A6116A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D36C79D3-5665-462C-8693-D77EB0172BA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" xr2:uid="{0EC3342C-DA2B-4212-93EF-7E4274CD2C90}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="34">
   <si>
     <t>Delta/Databricks Feature</t>
   </si>
@@ -662,6 +662,9 @@
       <c r="E8" t="s">
         <v>9</v>
       </c>
+      <c r="F8" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
@@ -767,6 +770,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="549332d9-68bf-4487-9fc8-f898b54ba2f4">
@@ -775,15 +787,6 @@
     <TaxCatchAll xmlns="e5446278-f595-413d-97e8-9d05bced5ef2" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1030,20 +1033,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FA90A2C-ECC6-4D8A-8320-8A9430408ADD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1518E235-21CD-4DD0-8F51-C8B7F1A485C0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="549332d9-68bf-4487-9fc8-f898b54ba2f4"/>
     <ds:schemaRef ds:uri="e5446278-f595-413d-97e8-9d05bced5ef2"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FA90A2C-ECC6-4D8A-8320-8A9430408ADD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>